<commit_message>
Update foul and swing rate logic
</commit_message>
<xml_diff>
--- a/Simulation/box_score.xlsx
+++ b/Simulation/box_score.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Team1_Batting" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Team2_Batting" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Team1_Pitching" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Team2_Pitching" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Team1_Batting" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Team2_Batting" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Team1_Pitching" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Team2_Pitching" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -496,51 +496,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Andrew Knizner</t>
+          <t>Mark Vientos</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H2" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.095</v>
+        <v>0.571</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nick Ahmed</t>
+          <t>Luken Baker</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -549,32 +549,32 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>20</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4</v>
+        <v>0.333</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.6</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CJ Abrams</t>
+          <t>Curtis Mead</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -592,13 +592,13 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.111</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -607,11 +607,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Matt Chapman</t>
+          <t>Hunter Feduccia</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -623,106 +623,106 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0.091</v>
+        <v>0.083</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Victor Robles</t>
+          <t>Andrew Benintendi</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.167</v>
+        <v>0.1</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ryan McMahon</t>
+          <t>Matt Thaiss</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>3</v>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>5</v>
-      </c>
       <c r="H7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I7" t="n">
-        <v>0.75</v>
+        <v>0.667</v>
       </c>
       <c r="J7" t="n">
-        <v>0.375</v>
+        <v>0.2</v>
       </c>
       <c r="K7" t="n">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Josh Jung</t>
+          <t>Colby Thomas</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -734,75 +734,75 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>2</v>
       </c>
       <c r="H8" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I8" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>0.111</v>
+        <v>0.091</v>
       </c>
       <c r="K8" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Christian Yelich</t>
+          <t>Gio Urshela</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.111</v>
+        <v>0.083</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ronald Acuña Jr.</t>
+          <t>Bryan Reynolds</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -811,19 +811,19 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I10" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0.167</v>
+        <v>0.059</v>
       </c>
       <c r="K10" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -905,88 +905,88 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jarred Kelenic</t>
+          <t>Tyrone Taylor</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I2" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.118</v>
+        <v>0.182</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Brendan Rodgers</t>
+          <t>Griffin Conine</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I3" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.111</v>
+        <v>0.188</v>
       </c>
       <c r="K3" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sam Haggerty</t>
+          <t>Marcelo Mayer</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -998,69 +998,69 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H4" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.308</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Eduardo Escobar</t>
+          <t>Michael Conforto</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="I5" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3</v>
+        <v>0.105</v>
       </c>
       <c r="K5" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Miguel Vargas</t>
+          <t>Alex Verdugo</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -1069,32 +1069,32 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I6" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="J6" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.5</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Luis Torrens</t>
+          <t>Leo Jiménez</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -1106,35 +1106,35 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>0.091</v>
+        <v>0.1</v>
       </c>
       <c r="K7" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Dane Myers</t>
+          <t>Jonathan Davis</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -1143,32 +1143,32 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H8" t="n">
         <v>9</v>
       </c>
       <c r="I8" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>0.111</v>
+        <v>0.222</v>
       </c>
       <c r="K8" t="n">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Colt Keith</t>
+          <t>Brandon Nimmo</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -1177,35 +1177,35 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I9" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.059</v>
+        <v>0.2</v>
       </c>
       <c r="K9" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Matt Shaw</t>
+          <t>Graham Pauley</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
@@ -1217,22 +1217,22 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
         <v>2</v>
       </c>
       <c r="H10" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I10" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J10" t="n">
-        <v>0.05</v>
+        <v>0.059</v>
       </c>
       <c r="K10" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1246,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1319,42 +1319,126 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Chris Sale</t>
+          <t>Clarke Schmidt</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>104</v>
+      </c>
+      <c r="J2" t="n">
+        <v>62</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>104-62</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jay Jackson</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
         <v>8</v>
       </c>
-      <c r="C2" t="n">
-        <v>12</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>12</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>111</v>
-      </c>
-      <c r="J2" t="n">
-        <v>76</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>111-76</t>
+      <c r="J3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>8-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Luis Medina</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>6</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>6-4</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1442,42 +1526,126 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ryne Stanek</t>
+          <t>Mike Clevinger</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>98</v>
+      </c>
+      <c r="J2" t="n">
+        <v>60</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>98-60</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>J.P. France</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>13</v>
+      </c>
+      <c r="J3" t="n">
+        <v>8</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>13-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ronny Henriquez</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>6</v>
       </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>112</v>
-      </c>
-      <c r="J2" t="n">
-        <v>76</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>112-76</t>
+      <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>6-4</t>
         </is>
       </c>
     </row>

</xml_diff>